<commit_message>
Noise UAM Test Updates
</commit_message>
<xml_diff>
--- a/03_Aircraft_Noise_Modeling/City_Simulations/UAM_City_Routes.xlsx
+++ b/03_Aircraft_Noise_Modeling/City_Simulations/UAM_City_Routes.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aidanmolloy/Documents/LEADS/RESEARCH/03_Aircraft_Noise_Modeling/City_Simulations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5F2A12-31AD-BE41-9922-A7A6FE96A060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93951E8D-3285-2E44-92E6-4039B4BEE3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="16940" xr2:uid="{0D3479EF-2BF9-A044-90EB-A477301D535B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Los Angeles" sheetId="1" r:id="rId1"/>
+    <sheet name="Los_Angeles" sheetId="1" r:id="rId1"/>
     <sheet name="San Francisco" sheetId="2" r:id="rId2"/>
     <sheet name="New York" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="73">
   <si>
     <t>Origin Code</t>
   </si>
@@ -251,6 +251,12 @@
   </si>
   <si>
     <t>−118.236962</t>
+  </si>
+  <si>
+    <t>Origin Latitude</t>
+  </si>
+  <si>
+    <t>Destination Latitude</t>
   </si>
 </sst>
 </file>
@@ -737,7 +743,7 @@
   <dimension ref="A1:L343"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.2"/>
@@ -754,7 +760,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
@@ -772,7 +778,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>8</v>

</xml_diff>